<commit_message>
NB Reporting: - kzt report 2 and 3 new forms (partial commit)
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_2.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_2.xlsx
@@ -18,7 +18,7 @@
     <definedName name="GR_CODE_ROW">4583</definedName>
     <definedName name="GR_CODE_SHEET">4</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ОПиУ_2!$A$1:$F$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">ОПиУ_2!$A$1:$F$49</definedName>
   </definedNames>
   <calcPr calcId="152511" iterateCount="10000" iterateDelta="1E-10"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Код формы</t>
   </si>
@@ -312,6 +312,57 @@
   </si>
   <si>
     <t>Прочие доходы (6210-6240, 6260, 6270, 6110.010, 6110.020, 6110.080, 6110.140, 6110.260, 6110.270, 6110.320, 6110.330, 6120, 6130, 6140, 6150.040, 6150.050,6160, 6280.040-6280.080, 6290, 6110.150, 6110.160, 6110.280-6110.310, 6400)</t>
+  </si>
+  <si>
+    <t>Доходы в виде вознаграждения по заемным операциям (6110.010, 6110.020, 6110.150, 6110.160)</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
   </si>
 </sst>
 </file>
@@ -532,6 +583,8 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -539,8 +592,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -860,10 +911,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,25 +1547,25 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
       <c r="G10" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1617,317 +1668,329 @@
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
-      <c r="B20" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="40">
-        <v>6</v>
+      <c r="B20" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>49</v>
       </c>
       <c r="D20" s="13"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="18"/>
-    </row>
-    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="40">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>50</v>
       </c>
       <c r="D21" s="13"/>
-      <c r="E21" s="11"/>
+      <c r="E21" s="17"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="40">
-        <v>8</v>
+        <v>21</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>51</v>
       </c>
       <c r="D22" s="13"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="H22" s="21"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E22" s="11"/>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="40">
-        <v>9</v>
+        <v>22</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>52</v>
       </c>
       <c r="D23" s="13"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="20"/>
-    </row>
-    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="H23" s="21"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="20"/>
+    </row>
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="40">
-        <v>10</v>
-      </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="38"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="40">
-        <v>11</v>
+      <c r="C25" s="40" t="s">
+        <v>54</v>
       </c>
       <c r="D25" s="13"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="20"/>
-    </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="E25" s="17"/>
+      <c r="F25" s="38"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="40">
-        <v>12</v>
+        <v>24</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>55</v>
       </c>
       <c r="D26" s="13"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="38"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E26" s="19"/>
+      <c r="F26" s="20"/>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="40">
-        <v>13</v>
+        <v>25</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="20"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="38"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
-      <c r="B28" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="40">
-        <v>14</v>
+      <c r="B28" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="40" t="s">
+        <v>57</v>
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="19"/>
       <c r="F28" s="20"/>
     </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="13"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="20"/>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="B30" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="40">
-        <v>15</v>
-      </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="38"/>
-      <c r="H29" s="21"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="42">
-        <v>16</v>
-      </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="48"/>
+      <c r="C30" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="38"/>
+      <c r="H30" s="21"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="23"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="45"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="B32" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="40">
-        <v>17</v>
-      </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="37"/>
-    </row>
-    <row r="32" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="22" t="s">
+      <c r="C32" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="13"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="37"/>
+    </row>
+    <row r="33" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="B33" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="42">
-        <v>18</v>
-      </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="24"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="40">
-        <v>19</v>
-      </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="37"/>
+      <c r="C33" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="23"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="24"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="37"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="42">
-        <v>20</v>
-      </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="25"/>
-    </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="23"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
-      <c r="B36" s="45" t="s">
+      <c r="B36" s="26"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="25"/>
+    </row>
+    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="25"/>
+      <c r="B37" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="46"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="45" t="s">
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="25"/>
+      <c r="B38" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-    </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="45" t="s">
+      <c r="C38" s="48"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="48"/>
+    </row>
+    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="25"/>
+      <c r="B39" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="46"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="29"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="48"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="29"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E40" s="21"/>
-      <c r="F40" s="30" t="s">
+      <c r="E41" s="21"/>
+      <c r="F41" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="G40" s="31"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="30"/>
-      <c r="C41" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="D41" s="30"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="32" t="s">
-        <v>40</v>
-      </c>
+      <c r="G41" s="31"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
+      <c r="C42" s="30" t="s">
+        <v>39</v>
+      </c>
       <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="32" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="E43" s="36" t="s">
-        <v>42</v>
-      </c>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
       <c r="F43" s="30"/>
       <c r="G43" s="31"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="33"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="32"/>
+      <c r="B44" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" s="30"/>
+      <c r="G44" s="31"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="34"/>
+      <c r="B45" s="33"/>
       <c r="C45" s="30"/>
       <c r="D45" s="30"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="32"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="31"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C47" s="31"/>
       <c r="D47" s="31"/>
       <c r="E47" s="31"/>
       <c r="F47" s="31"/>
-      <c r="G47" s="32"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="34"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
       <c r="F48" s="31"/>
       <c r="G48" s="32"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="34"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A10:F10"/>
-    <mergeCell ref="B36:F36"/>
     <mergeCell ref="B37:F37"/>
     <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="48" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
NB Reporting: - KZT Form 2 and 3 finished
</commit_message>
<xml_diff>
--- a/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_2.xlsx
+++ b/nicnbk-data/nicnbk-data-service-impl/src/main/resources/export_template/TEMPLATE_NICKMF_cons_KZT_2.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Код формы</t>
   </si>
@@ -111,41 +111,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Доходы в виде вознаграждения по размещенным вкладам </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">(6110.090-6110.130, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>6110.210-6110.250</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Доходы в виде вознаграждения по приобретенным ценным бумагам </t>
     </r>
     <r>
@@ -161,12 +126,6 @@
   </si>
   <si>
     <t>Доходы (расходы) от купли-продажи ценных бумаг (6280.010-6280.030, 7470.010-7470.030)</t>
-  </si>
-  <si>
-    <t>Доходы (расходы) от изменения стоимости ценных бумаг, оцениваемых по справедливой стоимости, изменения которой отражаются в составе прибыли или убытка (6150.010, 7330.010)</t>
-  </si>
-  <si>
-    <t>Доходы (расходы) от изменения стоимости ценных бумаг, имеющихся в наличии для продажи (6150.020, 6150.030, 7330.020, 7330.030)</t>
   </si>
   <si>
     <t>Доходы (расходы) от переоценки иностранной валюты (6250, 7430)</t>
@@ -198,21 +157,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Расходы в виде вознаграждения по полученным займам и финансовой аренде </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(7310.010-7310.040, 7310.080, 7310.090, 7310.190-7310.220, 7320.010)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Расходы по реализации </t>
     </r>
     <r>
@@ -228,12 +172,6 @@
   </si>
   <si>
     <t>Административные расходы (7210)</t>
-  </si>
-  <si>
-    <t>Прочие расходы (7310.050-7310.070, 7310.140-7310.180, 7310.230, 7310.240, 7330.040, 7330.050, 7340.010-7340.030, 7410, 7420, 7440-7460, 7470.040-7470.080, 7480, 7600)</t>
-  </si>
-  <si>
-    <t>Прибыль (убыток) до налогообложения (сумма строк 3-15)</t>
   </si>
   <si>
     <r>
@@ -251,9 +189,6 @@
     </r>
   </si>
   <si>
-    <t>Прибыль (убыток) после налогообложения от продолжающейся деятельности (сумма строк 16, 17)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Прибыль (убыток) от прекращенной деятельности </t>
     </r>
@@ -269,100 +204,70 @@
     </r>
   </si>
   <si>
-    <t>Чистая прибыль (убыток) (сумма строк 18, 19)</t>
-  </si>
-  <si>
-    <t>* В гр.1 четвертый знак номера счета указывается с учетом принадлежности к контрагентам (эмитентам), то есть от 1 до 3</t>
-  </si>
-  <si>
     <t>** Доходы указываются со знаком плюс, расходы указываются со знаком минус</t>
   </si>
   <si>
     <t>*** В гр. 4 указываются только контрагенты (эмитенты) Национальный Банк и дочерние организации Национального Банка</t>
   </si>
   <si>
-    <t xml:space="preserve">Руководитель </t>
-  </si>
-  <si>
-    <t>_________________</t>
-  </si>
-  <si>
-    <t>(фамилия и инициалы)</t>
-  </si>
-  <si>
-    <t>подпись</t>
-  </si>
-  <si>
-    <t>фамилия и номер телефона исполнителя</t>
-  </si>
-  <si>
     <t>Подписи скрепляются печатью</t>
   </si>
   <si>
     <t>Наименование организации: NICK Master Fund Ltd.</t>
   </si>
   <si>
-    <t>Рысбеков С.Д.</t>
-  </si>
-  <si>
     <t>по состоянию на дату</t>
   </si>
   <si>
     <t>&lt;dd.MM.yyyy&gt;</t>
   </si>
   <si>
-    <t>Прочие доходы (6210-6240, 6260, 6270, 6110.010, 6110.020, 6110.080, 6110.140, 6110.260, 6110.270, 6110.320, 6110.330, 6120, 6130, 6140, 6150.040, 6150.050,6160, 6280.040-6280.080, 6290, 6110.150, 6110.160, 6110.280-6110.310, 6400)</t>
-  </si>
-  <si>
     <t>Доходы в виде вознаграждения по заемным операциям (6110.010, 6110.020, 6110.150, 6110.160)</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>21</t>
+    <t>Прибыль (убыток) до налогообложения (сумма строк 3-16)</t>
+  </si>
+  <si>
+    <t>Прибыль (убыток) после налогообложения от продолжающейся деятельности (сумма строк 17, 18)</t>
+  </si>
+  <si>
+    <t>Чистая прибыль (убыток) (сумма строк 19, 20)</t>
+  </si>
+  <si>
+    <t>Примечание:* В гр.1 четвертый знак номера счета указывается с учетом принадлежности к контрагентам (эмитентам), то есть от 1 до 3</t>
+  </si>
+  <si>
+    <t>Руководитель              ____________________    ____________________ (подпись)</t>
+  </si>
+  <si>
+    <t>(имя, фамилия и отчество (при его наличии)</t>
+  </si>
+  <si>
+    <t>Главный бухгалтер    ____________________     ____________________ (подпись)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Исполнитель </t>
+  </si>
+  <si>
+    <t>____________________     ____________________ (подпись)</t>
+  </si>
+  <si>
+    <t>Доходы в виде вознаграждения по размещенным вкладам (6110.090-6110.110, 6110.220, 6110.230)</t>
+  </si>
+  <si>
+    <t>Доходы (расходы) от изменения стоимости ценных бумаг, оцениваемых по справедливой стоимости через прибыль или убыток (6150.010, 7330.010)</t>
+  </si>
+  <si>
+    <t>Доходы (расходы) от изменения стоимости ценных бумаг, оцениваемых по справедливой стоимости через прочий совокупный доход (6150.020, 6150.030, 7330.020, 7330.030)</t>
+  </si>
+  <si>
+    <t>Прочие доходы (6210-6240, 6260, 6110.080, 6110.320, 6110.330, 6110.340, 6110.350, 6120, 6130, 6140, 6150.060, 6160.030, 6170, 6280.060-6280.080, 6280.100, 6110.280-6110.310, 6400)</t>
+  </si>
+  <si>
+    <t>Расходы в виде вознаграждения по заемным операциям и аренде (7310.010-7310.040, 7310.080, 7310.090, 7310.190-7310.220, 7320.010)</t>
+  </si>
+  <si>
+    <t>Прочие расходы (7310.050-7310.070, 7310.150-7310.160, 7310.230, 7310.240, 7310.250, 7330.060, 7340.030, 7410, 7420, 7440, 7470.060-7470.090, 7350, 7600)</t>
   </si>
 </sst>
 </file>
@@ -375,7 +280,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.0000_р_._-;\-* #,##0.0000_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.000_р_._-;\-* #,##0.000_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,6 +349,19 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -477,12 +395,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -557,15 +476,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -573,28 +485,31 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 7" xfId="3"/>
     <cellStyle name="Обычный_ФормОтчет" xfId="2"/>
     <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
   </cellStyles>
@@ -913,8 +828,8 @@
   </sheetPr>
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,8 +1427,8 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="43" t="s">
-        <v>46</v>
+      <c r="C2" s="38" t="s">
+        <v>31</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>4</v>
@@ -1543,29 +1458,29 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
+      <c r="A10" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
       <c r="G10" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1613,7 +1528,7 @@
       <c r="B15" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="40">
+      <c r="C15" s="43">
         <v>1</v>
       </c>
       <c r="D15" s="13"/>
@@ -1625,7 +1540,7 @@
       <c r="B16" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="40">
+      <c r="C16" s="43">
         <v>2</v>
       </c>
       <c r="D16" s="13"/>
@@ -1637,7 +1552,7 @@
       <c r="B17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="41">
+      <c r="C17" s="44">
         <v>3</v>
       </c>
       <c r="D17" s="15"/>
@@ -1647,9 +1562,9 @@
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="40">
+        <v>42</v>
+      </c>
+      <c r="C18" s="43">
         <v>4</v>
       </c>
       <c r="D18" s="13"/>
@@ -1659,9 +1574,9 @@
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="40">
+        <v>18</v>
+      </c>
+      <c r="C19" s="43">
         <v>5</v>
       </c>
       <c r="D19" s="13"/>
@@ -1671,10 +1586,10 @@
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="40" t="s">
-        <v>49</v>
+        <v>32</v>
+      </c>
+      <c r="C20" s="43">
+        <v>6</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="11"/>
@@ -1683,22 +1598,22 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>50</v>
+        <v>19</v>
+      </c>
+      <c r="C21" s="43">
+        <v>7</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="17"/>
       <c r="F21" s="18"/>
     </row>
-    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>51</v>
+        <v>43</v>
+      </c>
+      <c r="C22" s="43">
+        <v>8</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="11"/>
@@ -1707,10 +1622,10 @@
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="40" t="s">
-        <v>52</v>
+        <v>44</v>
+      </c>
+      <c r="C23" s="43">
+        <v>9</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="17"/>
@@ -1720,34 +1635,34 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="40" t="s">
-        <v>53</v>
+        <v>20</v>
+      </c>
+      <c r="C24" s="43">
+        <v>10</v>
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="19"/>
       <c r="F24" s="20"/>
     </row>
-    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="40" t="s">
-        <v>54</v>
+        <v>45</v>
+      </c>
+      <c r="C25" s="43">
+        <v>11</v>
       </c>
       <c r="D25" s="13"/>
       <c r="E25" s="17"/>
-      <c r="F25" s="38"/>
+      <c r="F25" s="36"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>55</v>
+        <v>21</v>
+      </c>
+      <c r="C26" s="43">
+        <v>12</v>
       </c>
       <c r="D26" s="13"/>
       <c r="E26" s="19"/>
@@ -1756,22 +1671,22 @@
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="40" t="s">
-        <v>56</v>
+        <v>46</v>
+      </c>
+      <c r="C27" s="43">
+        <v>13</v>
       </c>
       <c r="D27" s="13"/>
       <c r="E27" s="17"/>
-      <c r="F27" s="38"/>
+      <c r="F27" s="36"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="40" t="s">
-        <v>57</v>
+        <v>22</v>
+      </c>
+      <c r="C28" s="43">
+        <v>14</v>
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="19"/>
@@ -1780,10 +1695,10 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="40" t="s">
-        <v>58</v>
+        <v>23</v>
+      </c>
+      <c r="C29" s="43">
+        <v>15</v>
       </c>
       <c r="D29" s="13"/>
       <c r="E29" s="19"/>
@@ -1792,76 +1707,76 @@
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="40" t="s">
-        <v>59</v>
+        <v>47</v>
+      </c>
+      <c r="C30" s="43">
+        <v>16</v>
       </c>
       <c r="D30" s="13"/>
       <c r="E30" s="17"/>
-      <c r="F30" s="38"/>
+      <c r="F30" s="36"/>
       <c r="H30" s="21"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="42" t="s">
-        <v>60</v>
+        <v>33</v>
+      </c>
+      <c r="C31" s="44">
+        <v>17</v>
       </c>
       <c r="D31" s="23"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="45"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="40"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" s="40" t="s">
-        <v>61</v>
+        <v>24</v>
+      </c>
+      <c r="C32" s="43">
+        <v>18</v>
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="19"/>
-      <c r="F32" s="37"/>
+      <c r="F32" s="35"/>
     </row>
     <row r="33" spans="1:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="42" t="s">
-        <v>62</v>
+        <v>34</v>
+      </c>
+      <c r="C33" s="44">
+        <v>19</v>
       </c>
       <c r="D33" s="23"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="45"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="40"/>
       <c r="G33" s="24"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="40" t="s">
-        <v>63</v>
+        <v>25</v>
+      </c>
+      <c r="C34" s="43">
+        <v>20</v>
       </c>
       <c r="D34" s="13"/>
       <c r="E34" s="19"/>
-      <c r="F34" s="37"/>
+      <c r="F34" s="35"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="42" t="s">
-        <v>64</v>
+        <v>35</v>
+      </c>
+      <c r="C35" s="44">
+        <v>21</v>
       </c>
       <c r="D35" s="23"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="45"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="40"/>
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
     </row>
@@ -1870,38 +1785,38 @@
       <c r="B36" s="26"/>
       <c r="C36" s="27"/>
       <c r="D36" s="27"/>
-      <c r="E36" s="39"/>
+      <c r="E36" s="37"/>
       <c r="F36" s="25"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="48"/>
+      <c r="A37" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="46"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" s="48"/>
-      <c r="D38" s="48"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="48"/>
+      <c r="A38" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="46"/>
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
+      <c r="A39" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="46"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" s="28"/>
@@ -1910,77 +1825,89 @@
       <c r="E40" s="29"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="30"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="31"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E41" s="21"/>
-      <c r="F41" s="30" t="s">
+      <c r="B42" s="42"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="41"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="32"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="41"/>
+      <c r="B43" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="G41" s="31"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="30"/>
-      <c r="C42" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="D42" s="30"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
       <c r="E43" s="30"/>
       <c r="F43" s="30"/>
       <c r="G43" s="31"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="E44" s="36" t="s">
-        <v>42</v>
-      </c>
+      <c r="A44" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" s="42"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="34"/>
       <c r="F44" s="30"/>
       <c r="G44" s="31"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="33"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="41"/>
+      <c r="D45" s="41"/>
       <c r="E45" s="31"/>
       <c r="F45" s="32"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="34"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
+      <c r="A46" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" s="41"/>
+      <c r="D46" s="41"/>
       <c r="E46" s="30"/>
       <c r="F46" s="30"/>
       <c r="G46" s="31"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
+      <c r="A47" s="41"/>
+      <c r="B47" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
       <c r="E47" s="31"/>
       <c r="F47" s="31"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
+      <c r="A48" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="42"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="41"/>
       <c r="E48" s="31"/>
       <c r="F48" s="31"/>
       <c r="G48" s="32"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="34"/>
+      <c r="B49" s="33"/>
       <c r="F49" s="31"/>
       <c r="G49" s="32"/>
     </row>
@@ -1988,9 +1915,9 @@
   <mergeCells count="5">
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A10:F10"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A39:F39"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="48" orientation="portrait" r:id="rId1"/>

</xml_diff>